<commit_message>
add download template option
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C2F48E-1B5C-478B-9CA5-D6BA866CF2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FC03AB-98BB-47F3-A88D-34778E3A74D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="396" windowWidth="17280" windowHeight="8976" activeTab="3" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="384" yWindow="396" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Voertuig</t>
   </si>
@@ -108,13 +108,43 @@
   </si>
   <si>
     <t>locatie</t>
+  </si>
+  <si>
+    <t>2023-01-02 07:22</t>
+  </si>
+  <si>
+    <t>2023-01-02 07:23</t>
+  </si>
+  <si>
+    <t>2023-01-02 09:02</t>
+  </si>
+  <si>
+    <t>2023-01-02 09:14</t>
+  </si>
+  <si>
+    <t>2023-01-02 11:22</t>
+  </si>
+  <si>
+    <t>2023-01-02 12:14</t>
+  </si>
+  <si>
+    <t>2023-01-02 14:51</t>
+  </si>
+  <si>
+    <t>2023-01-02 15:26</t>
+  </si>
+  <si>
+    <t>2023-01-02 17:52</t>
+  </si>
+  <si>
+    <t>2023-01-03 07:02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,31 +153,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,13 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,14 +499,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581F7C9C-3D18-4DAF-B1AF-13B070A46206}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -516,182 +528,182 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>44958.307337962964</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44958.308032407411</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44958.308032407411</v>
-      </c>
-      <c r="C3" s="2">
-        <v>44958.376828703702</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44958.376828703702</v>
-      </c>
-      <c r="C4" s="2">
-        <v>44958.385138888887</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <v>44958.385138888887</v>
-      </c>
-      <c r="C5" s="2">
-        <v>44958.473819444444</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>124</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>44958.473819444444</v>
-      </c>
-      <c r="C6" s="2">
-        <v>44958.510208333333</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44958.510208333333</v>
-      </c>
-      <c r="C7" s="2">
-        <v>44958.619386574072</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>133</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>44958.619386574072</v>
-      </c>
-      <c r="C8" s="2">
-        <v>44958.643194444441</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <v>44958.643194444441</v>
-      </c>
-      <c r="C9" s="2">
-        <v>44958.745115740741</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>167</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>44958.745115740741</v>
-      </c>
-      <c r="C10" s="2">
-        <v>44959.293402777781</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -706,7 +718,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,58 +727,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
     </row>
@@ -777,10 +789,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC7A104-0D62-4335-A3C9-D751C0741FE0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,36 +801,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>44</v>
       </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -827,28 +843,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91913FF-1F61-453A-9639-D48ABF42F8BA}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change column name in template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC233469-C0D8-4972-9C61-703648826CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC38D7C-FA9C-4F03-A7D5-8DB2469B7CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="744" windowWidth="17280" windowHeight="8976" activeTab="2" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="732" yWindow="744" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581F7C9C-3D18-4DAF-B1AF-13B070A46206}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC7A104-0D62-4335-A3C9-D751C0741FE0}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
change column name in template2
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC38D7C-FA9C-4F03-A7D5-8DB2469B7CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2025DD-AC0C-4439-AC60-1806DD9E5984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="744" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="384" yWindow="396" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
add parameter configuration from input file
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2025DD-AC0C-4439-AC60-1806DD9E5984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F8F7DD-B637-41E4-9AD2-384AE4A5C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="396" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="732" yWindow="744" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>
@@ -866,7 +866,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add second vehicle to template and change table format of activiteiten sheet
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F8F7DD-B637-41E4-9AD2-384AE4A5C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C543E7BC-1A72-4D9B-B84E-569D451B9A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="744" windowWidth="17280" windowHeight="8976" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="588" yWindow="372" windowWidth="21396" windowHeight="10668" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Voertuig</t>
   </si>
@@ -83,12 +83,6 @@
     <t>Loscontainer Opzetten</t>
   </si>
   <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>Laden</t>
-  </si>
-  <si>
     <t>Pauze</t>
   </si>
   <si>
@@ -138,6 +132,24 @@
   </si>
   <si>
     <t>efficiency</t>
+  </si>
+  <si>
+    <t>parkeerplaats A12</t>
+  </si>
+  <si>
+    <t>2023-01-02 06:55</t>
+  </si>
+  <si>
+    <t>2023-01-02 11:05</t>
+  </si>
+  <si>
+    <t>2023-01-02 12:31</t>
+  </si>
+  <si>
+    <t>2023-01-02 15:12</t>
+  </si>
+  <si>
+    <t>2023-01-03 07:48</t>
   </si>
 </sst>
 </file>
@@ -179,10 +191,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +513,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,10 +547,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -554,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -574,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -594,10 +607,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -614,19 +627,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -634,13 +647,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1">
         <v>133</v>
@@ -653,13 +666,13 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1">
@@ -673,13 +686,13 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1">
@@ -693,13 +706,13 @@
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1">
@@ -710,36 +723,84 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>150</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1">
+        <v>150</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -789,10 +850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B17DB9-DF25-4A63-B4B3-4A4BD3FEA471}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,60 +861,29 @@
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -876,15 +906,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>300</v>
@@ -892,7 +922,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>600</v>
@@ -900,7 +930,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>44</v>
@@ -908,7 +938,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>1.25</v>

</xml_diff>

<commit_message>
add laadvermogen snelweg to template and improvement of demand plot
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C543E7BC-1A72-4D9B-B84E-569D451B9A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21120EC-71D6-4EDA-AE05-48FAACC9FF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="372" windowWidth="21396" windowHeight="10668" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Voertuig</t>
   </si>
@@ -98,9 +98,6 @@
     <t>aansluittijd</t>
   </si>
   <si>
-    <t>laadvermogen</t>
-  </si>
-  <si>
     <t>2023-01-02 07:22</t>
   </si>
   <si>
@@ -137,19 +134,25 @@
     <t>parkeerplaats A12</t>
   </si>
   <si>
-    <t>2023-01-02 06:55</t>
-  </si>
-  <si>
-    <t>2023-01-02 11:05</t>
-  </si>
-  <si>
-    <t>2023-01-02 12:31</t>
-  </si>
-  <si>
-    <t>2023-01-02 15:12</t>
-  </si>
-  <si>
-    <t>2023-01-03 07:48</t>
+    <t>laadvermogen bedrijf</t>
+  </si>
+  <si>
+    <t>laadvermogen snelweg</t>
+  </si>
+  <si>
+    <t>2023-01-03 06:55</t>
+  </si>
+  <si>
+    <t>2023-01-03 11:05</t>
+  </si>
+  <si>
+    <t>2023-01-03 12:31</t>
+  </si>
+  <si>
+    <t>2023-01-03 15:12</t>
+  </si>
+  <si>
+    <t>2023-01-04 07:48</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,10 +529,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -546,11 +549,11 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -566,11 +569,11 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -586,11 +589,11 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -606,11 +609,11 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -626,14 +629,14 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -646,14 +649,14 @@
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>133</v>
@@ -667,10 +670,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -687,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
@@ -707,10 +710,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -727,16 +730,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
@@ -747,14 +750,12 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="1">
         <v>0</v>
       </c>
@@ -767,16 +768,14 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -787,10 +786,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -804,40 +803,40 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -893,15 +892,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC7A104-0D62-4335-A3C9-D751C0741FE0}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,7 +929,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>44</v>
@@ -938,9 +937,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
         <v>1.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Download template algemeen gemaakt
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin Buijs\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B91BAC5-73AC-4A24-8D43-BB59B3648CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B306266-CE00-415D-923A-B93B4E987224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B9C36790-AB44-4751-B982-A88CE4B8AE35}"/>
   </bookViews>
   <sheets>
     <sheet name="ritten" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581F7C9C-3D18-4DAF-B1AF-13B070A46206}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -922,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91913FF-1F61-453A-9639-D48ABF42F8BA}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>